<commit_message>
Added info and columns added to dataset file
</commit_message>
<xml_diff>
--- a/inst/app/data/sale_app_data_list.xlsx
+++ b/inst/app/data/sale_app_data_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,16 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>Data set</t>
-  </si>
-  <si>
-    <t>Condition 1</t>
-  </si>
-  <si>
-    <t>Condition 2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Cerebral Organoids day 40</t>
   </si>
@@ -52,6 +43,24 @@
   </si>
   <si>
     <t>tables/tendon vs PSC.xlsx</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Condition1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tendons vs PSC </t>
+  </si>
+  <si>
+    <t>Cerebral Organoids day 40 compared to hPSC and this is a very long wall of text. I write a few more words to make it even longer</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Condition2</t>
   </si>
 </sst>
 </file>
@@ -385,62 +394,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="36" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="E3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned the ui file
</commit_message>
<xml_diff>
--- a/inst/app/data/sale_app_data_list.xlsx
+++ b/inst/app/data/sale_app_data_list.xlsx
@@ -54,13 +54,13 @@
     <t xml:space="preserve">Tendons vs PSC </t>
   </si>
   <si>
-    <t>Cerebral Organoids day 40 compared to hPSC and this is a very long wall of text. I write a few more words to make it even longer</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>Condition2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cerebral Organoids day 40 compared to hPSC and this is a long wall of text. I write a few more words to make it even longer. This shows that we can have a very verbose description of the data set amd it wil stil be displayed correctly in the app. </t>
   </si>
 </sst>
 </file>
@@ -397,7 +397,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,13 +414,13 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>

</xml_diff>